<commit_message>
Ids to Slice. Conjunto enviado ao Marcelo
</commit_message>
<xml_diff>
--- a/src/site/ids to Slicer.xlsx
+++ b/src/site/ids to Slicer.xlsx
@@ -105,8 +105,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -384,7 +412,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,9 +483,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">

</xml_diff>